<commit_message>
Process excel sheet on the heals of validating
branch:
</commit_message>
<xml_diff>
--- a/tests/test_resources/output_person/test_namescan-explained.xlsx
+++ b/tests/test_resources/output_person/test_namescan-explained.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>17750593383858545464</t>
+          <t>5465859685115260427</t>
         </is>
       </c>
       <c r="J2" t="b">
@@ -594,7 +594,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>9565943872225982104</t>
+          <t>5527442777154739395</t>
         </is>
       </c>
       <c r="J3" t="b">
@@ -645,7 +645,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1382086158180223442</t>
+          <t>11048837401662965790</t>
         </is>
       </c>
       <c r="J4" t="b">
@@ -705,7 +705,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>5744382305461071716</t>
+          <t>17311461800651806091</t>
         </is>
       </c>
       <c r="J5" t="b">
@@ -771,7 +771,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>8857692561240401991</t>
+          <t>10171788987322014488</t>
         </is>
       </c>
       <c r="J6" t="b">
@@ -827,7 +827,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>11428755131739180661</t>
+          <t>1640453089486844230</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -874,7 +874,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>14570658688989279644</t>
+          <t>15186096852338279725</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -925,7 +925,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>9789653759455730552</t>
+          <t>18437259150481094143</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -972,7 +972,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2227794423361950601</t>
+          <t>1975812593444422882</t>
         </is>
       </c>
       <c r="J10" t="b">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>16064591688497546577</t>
+          <t>17220968564977943993</t>
         </is>
       </c>
       <c r="J11" t="b">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>5361364709157549748</t>
+          <t>9851901183800940666</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>13197035708448077581</t>
+          <t>4651596805960560616</t>
         </is>
       </c>
       <c r="J13" t="b">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2642283516059678581</t>
+          <t>5363012115113112816</t>
         </is>
       </c>
       <c r="J14" t="b">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>10904643773617528460</t>
+          <t>12127878054617990148</t>
         </is>
       </c>
       <c r="J15" t="b">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>13546369845597778697</t>
+          <t>12615781559068715528</t>
         </is>
       </c>
       <c r="J16" t="b">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>12612806687587669465</t>
+          <t>16379321365746720216</t>
         </is>
       </c>
       <c r="J17" t="b">
@@ -1399,7 +1399,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>15519997683086084107</t>
+          <t>1859052510171157074</t>
         </is>
       </c>
       <c r="J18" t="b">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>16486547996799273751</t>
+          <t>131388509170113531</t>
         </is>
       </c>
       <c r="J19" t="b">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>17661703409476697691</t>
+          <t>12276360953888945774</t>
         </is>
       </c>
       <c r="J20" t="b">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>17840573855974732220</t>
+          <t>17948212404227027011</t>
         </is>
       </c>
       <c r="J21" t="b">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>16916979888425215825</t>
+          <t>1777086285660115289</t>
         </is>
       </c>
       <c r="J22" t="b">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>3418160615949916528</t>
+          <t>17550978780941298109</t>
         </is>
       </c>
       <c r="J23" t="b">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>8010919983063203789</t>
+          <t>2131671840104369538</t>
         </is>
       </c>
       <c r="J24" t="b">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>5737178164591258820</t>
+          <t>646713366152604332</t>
         </is>
       </c>
       <c r="J25" t="b">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>10722991830633008318</t>
+          <t>10373905228459429881</t>
         </is>
       </c>
       <c r="J26" t="b">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>306588275765262214</t>
+          <t>4258573009579735995</t>
         </is>
       </c>
       <c r="J27" t="b">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>12728213663946471115</t>
+          <t>265240268283751376</t>
         </is>
       </c>
       <c r="J28" t="b">
@@ -1950,7 +1950,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>8427673938370929927</t>
+          <t>1716153287694692260</t>
         </is>
       </c>
       <c r="J29" t="b">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>15211200567548200615</t>
+          <t>7011195061182511990</t>
         </is>
       </c>
       <c r="J30" t="b">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>5966139624153910373</t>
+          <t>9986674937439859568</t>
         </is>
       </c>
       <c r="J31" t="b">
@@ -2103,7 +2103,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>4605239560544824555</t>
+          <t>8924521215966159335</t>
         </is>
       </c>
       <c r="J32" t="b">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>6095673613569968877</t>
+          <t>6389173515177744956</t>
         </is>
       </c>
       <c r="J33" t="b">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>12241321737361704499</t>
+          <t>14148993971580128743</t>
         </is>
       </c>
       <c r="J34" t="b">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>9906367740922092012</t>
+          <t>583765279824930520</t>
         </is>
       </c>
       <c r="J35" t="b">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>5373983457554281357</t>
+          <t>10837231579467459848</t>
         </is>
       </c>
       <c r="J36" t="b">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>17869940490237480164</t>
+          <t>10363795271348284161</t>
         </is>
       </c>
       <c r="J37" t="b">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>11658978149433584496</t>
+          <t>15523820850506490992</t>
         </is>
       </c>
       <c r="J38" t="b">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>17779181313092304073</t>
+          <t>5227751510528346188</t>
         </is>
       </c>
       <c r="J39" t="b">
@@ -2487,7 +2487,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>11136595241382493197</t>
+          <t>7485263210229603469</t>
         </is>
       </c>
       <c r="J40" t="b">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>7710133813911121244</t>
+          <t>15481276480988585061</t>
         </is>
       </c>
       <c r="J41" t="b">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>6412000219855483793</t>
+          <t>11770231653918674322</t>
         </is>
       </c>
       <c r="J42" t="b">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>8514953095007454381</t>
+          <t>13819626741178253463</t>
         </is>
       </c>
       <c r="J43" t="b">
@@ -2688,7 +2688,7 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>16015874943614749943</t>
+          <t>13396730022424409992</t>
         </is>
       </c>
       <c r="J44" t="b">
@@ -2735,7 +2735,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>16558349590308473239</t>
+          <t>2523881632023293484</t>
         </is>
       </c>
       <c r="J45" t="b">
@@ -2782,7 +2782,7 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>11677539966015143473</t>
+          <t>10587417906698095327</t>
         </is>
       </c>
       <c r="J46" t="b">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>884237522075041945</t>
+          <t>9033843866905793904</t>
         </is>
       </c>
       <c r="J47" t="b">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>13157580395453485236</t>
+          <t>8368446460655908217</t>
         </is>
       </c>
       <c r="J48" t="b">
@@ -2927,7 +2927,7 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>6815454968028151454</t>
+          <t>2448008120671130484</t>
         </is>
       </c>
       <c r="J49" t="b">
@@ -2974,7 +2974,7 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>14585109624729361171</t>
+          <t>676658871738576226</t>
         </is>
       </c>
       <c r="J50" t="b">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>9248276871841134283</t>
+          <t>11815689254016262160</t>
         </is>
       </c>
       <c r="J51" t="b">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2658927807518344464</t>
+          <t>1865281822864486586</t>
         </is>
       </c>
       <c r="J52" t="b">
@@ -3119,7 +3119,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>7433175588447306402</t>
+          <t>11999168590972673814</t>
         </is>
       </c>
       <c r="J53" t="b">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>17454329067522470126</t>
+          <t>15663199238863036415</t>
         </is>
       </c>
       <c r="J54" t="b">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>18031490626720554929</t>
+          <t>3482048972607296362</t>
         </is>
       </c>
       <c r="J55" t="b">
@@ -3268,7 +3268,7 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>866446762336077001</t>
+          <t>9297669140363783287</t>
         </is>
       </c>
       <c r="J56" t="b">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>1505875663710161889</t>
+          <t>825577570103515494</t>
         </is>
       </c>
       <c r="J57" t="b">
@@ -3362,7 +3362,7 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>13938151234672454859</t>
+          <t>17077985264131744185</t>
         </is>
       </c>
       <c r="J58" t="b">
@@ -3409,7 +3409,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>13363227029108424371</t>
+          <t>2590433911241102872</t>
         </is>
       </c>
       <c r="J59" t="b">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>2424300356184703538</t>
+          <t>583355402538321026</t>
         </is>
       </c>
       <c r="J60" t="b">
@@ -3507,7 +3507,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>3553623342203872443</t>
+          <t>389810736453788751</t>
         </is>
       </c>
       <c r="J61" t="b">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>16101687572041719502</t>
+          <t>7050301517988511742</t>
         </is>
       </c>
       <c r="J62" t="b">
@@ -3609,7 +3609,7 @@
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>17647502611624314989</t>
+          <t>12641924004534609258</t>
         </is>
       </c>
       <c r="J63" t="b">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>15192644702245681928</t>
+          <t>9056830240370997859</t>
         </is>
       </c>
       <c r="J64" t="b">
@@ -3703,7 +3703,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>13643938760245206863</t>
+          <t>13942523387772293193</t>
         </is>
       </c>
       <c r="J65" t="b">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>12465649417542391245</t>
+          <t>15832826006729248969</t>
         </is>
       </c>
       <c r="J66" t="b">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>15162945499940540343</t>
+          <t>13355582891255512253</t>
         </is>
       </c>
       <c r="J67" t="b">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>15682162917236121729</t>
+          <t>17377645535285548270</t>
         </is>
       </c>
       <c r="J68" t="b">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>6263128611681725473</t>
+          <t>6897379166409132309</t>
         </is>
       </c>
       <c r="J69" t="b">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>11337239569067802468</t>
+          <t>16292580299745028902</t>
         </is>
       </c>
       <c r="J70" t="b">
@@ -3985,7 +3985,7 @@
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>5458063160365920116</t>
+          <t>4397641155899062092</t>
         </is>
       </c>
       <c r="J71" t="b">

</xml_diff>